<commit_message>
otra caracteristica agregada :V
</commit_message>
<xml_diff>
--- a/Construccion.xlsx
+++ b/Construccion.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>Identificador</t>
   </si>
@@ -109,7 +109,10 @@
     <t>Complementando la caracteristica 9 el cliente podra reservar meseros</t>
   </si>
   <si>
-    <t>complementando la caracteristica 18 el cliente pueda ver la calificacion de dicha comida</t>
+    <t>Complementando la caracteristica 18 el cliente pueda ver la calificacion de dicha comida</t>
+  </si>
+  <si>
+    <t>Complementando a la caracteristica 2 la pagina tambien puede mostrar la calificacion del restaurante</t>
   </si>
 </sst>
 </file>
@@ -434,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -714,6 +717,12 @@
     <row r="25" spans="1:3">
       <c r="A25">
         <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:3">

</xml_diff>